<commit_message>
update gon-evidence B1 B2
</commit_message>
<xml_diff>
--- a/PetrFerz/evidence.xlsx
+++ b/PetrFerz/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="13176" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="13176" firstSheet="1" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="74">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -251,6 +251,18 @@
   </si>
   <si>
     <t>9DF81D10FC20DA1AB83F5EDD7C50DBB41F3E3325F1D16BC9F577681F5957663C</t>
+  </si>
+  <si>
+    <t>750930A99EA0FB5D058B007F54126EAA9D9E10876FD4E3953AF73457C60CD1F8</t>
+  </si>
+  <si>
+    <t>39BCDD4F4DF21C3232C67438E9CAB45B512212BC5B1665B28D086E457B27FF26</t>
+  </si>
+  <si>
+    <t>E23C59B962D4FDCA69E1EBA4C64BC8651AD9F4EC77E8FD925DD9F88CBF882432</t>
+  </si>
+  <si>
+    <t>3DCE927D8B3BBDF8B2CEF4E00424E5E40DFCE4336F7C0A46B90D5B46987534D8</t>
   </si>
 </sst>
 </file>
@@ -3123,7 +3135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -3595,7 +3607,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3614,7 +3628,7 @@
     </row>
     <row r="2" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3623,7 +3637,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -3693,7 +3707,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3712,7 +3728,7 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3721,7 +3737,7 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>

</xml_diff>

<commit_message>
edits for A2-A6 , add B5-B7
</commit_message>
<xml_diff>
--- a/PetrFerz/evidence.xlsx
+++ b/PetrFerz/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="13176" firstSheet="1" activeTab="23"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="13176" firstSheet="1" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -33,13 +33,14 @@
     <sheet name="B2" sheetId="24" r:id="rId24"/>
     <sheet name="B5" sheetId="25" r:id="rId25"/>
     <sheet name="B6" sheetId="26" r:id="rId26"/>
+    <sheet name="B7" sheetId="27" r:id="rId27"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="126">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -104,18 +105,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>A4</t>
   </si>
   <si>
     <t>A5</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
     <t>A6</t>
   </si>
   <si>
@@ -140,15 +135,6 @@
     <t>A13</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>A14</t>
   </si>
   <si>
@@ -173,12 +159,6 @@
     <t>B1</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>B2</t>
   </si>
   <si>
@@ -189,11 +169,11 @@
   </si>
   <si>
     <t>elgafar-1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>uptick_7000-2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>PetrFerz</t>
@@ -223,36 +203,12 @@
     <t>petrferz</t>
   </si>
   <si>
-    <t>E512C9A8EA6470D6AD8C5724DB6483C5A68FCD7CE0100F5356B495BB6C9ECE8E</t>
-  </si>
-  <si>
-    <t>nft3</t>
-  </si>
-  <si>
-    <t>A484B8CD091A1A72C869C1968C457386260D28A5D27BA88C8BB3B03FDF9B3151</t>
-  </si>
-  <si>
-    <t>nft4</t>
-  </si>
-  <si>
-    <t>1A5428700BD17A6D27A19949A54155F8025681BCEF66D33DD44547CD1290C324</t>
-  </si>
-  <si>
     <t>stars1qtxp7z8zq2e9v86cra29dfext6yplt86fpuay9zghq32uv6j3w7qy2aqfn</t>
   </si>
   <si>
-    <t>85BC06C4B7AA850DFC3036604DB4229B1261B04888345DAFEA92E426499749A5</t>
-  </si>
-  <si>
     <t>ibc/C1EBE6217000CD8AE246B19728AF084709B12115181BA2AE5A6A4E159DB886AA</t>
   </si>
   <si>
-    <t>4EC9BD8F23928BC01E81A1761A8B52F5B2DB715DA9C826274BAFE4EAAF348F6E</t>
-  </si>
-  <si>
-    <t>9DF81D10FC20DA1AB83F5EDD7C50DBB41F3E3325F1D16BC9F577681F5957663C</t>
-  </si>
-  <si>
     <t>750930A99EA0FB5D058B007F54126EAA9D9E10876FD4E3953AF73457C60CD1F8</t>
   </si>
   <si>
@@ -263,17 +219,226 @@
   </si>
   <si>
     <t>3DCE927D8B3BBDF8B2CEF4E00424E5E40DFCE4336F7C0A46B90D5B46987534D8</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>nftstage2A7</t>
+  </si>
+  <si>
+    <t>nftstage2A8</t>
+  </si>
+  <si>
+    <t>nftstage2A9</t>
+  </si>
+  <si>
+    <t>nftstage2A10</t>
+  </si>
+  <si>
+    <t>nftstage2A11</t>
+  </si>
+  <si>
+    <t>nftstage2A12</t>
+  </si>
+  <si>
+    <t>ibc/7B242D561D6B9D6CBF67FE5A6ABAE469E4B7A4E0391E8DCE3C907C75699D029D</t>
+  </si>
+  <si>
+    <t>ibc/7AC5EFF97768D8B89B2F4A7C6ABF874D139EDF471FBD9CA1E1CB5F8225872158</t>
+  </si>
+  <si>
+    <t>ibc/E89D7F725B83732571230E24E0646E3BE5D55224D880DE008A16A4E735E5F75A</t>
+  </si>
+  <si>
+    <t>ibc/25489D9ECFC1BF8C5561F50B9B6CABF0EED17503DB0B11361E65388BA8255F93</t>
+  </si>
+  <si>
+    <t>ibc/1CC3715D8CE7AD0249BA57EAFBF302B6174D661A2454EB94C26B4D3FD35197FD</t>
+  </si>
+  <si>
+    <t>ibc/C4096A5F04FF24E9E01CF84788C60CA5DAAA30C13A51FDF5E60C8D915703AF16</t>
+  </si>
+  <si>
+    <t>7053DF13339C4CE36827D9E062AC585E048770AE4AEB9B1F565495441B916AB0</t>
+  </si>
+  <si>
+    <t>77CE759DF68606B92A804F1E25488581B8AE0FDA77413E0FEC0EF8004B4A16C9</t>
+  </si>
+  <si>
+    <t>7790354575083980C966628307763B5433A383CBC077C0BE9B3ED62AE1407DB6</t>
+  </si>
+  <si>
+    <t>A9D28CCE85BDAB76E13F86E0ADD0DA0B482B1C520697795992A19B579813E58D</t>
+  </si>
+  <si>
+    <t>130AD8F717EB63D83AED537A22282FE1FE64BB5E1E07D4C528006D040AC3184C</t>
+  </si>
+  <si>
+    <t>58559468F1044F546B19CC9C0DED503453D4FCED1978D742E3143AA8BACD6FCC</t>
+  </si>
+  <si>
+    <t>D36153FA9FFB61B8B0A3EBB1B0E2E7FF84FC3C33FE20C1AB42AC30F6C427A977</t>
+  </si>
+  <si>
+    <t>F2D578BB2611D8463D37C5D0537DBE82C4E63151100423B3C9A4027254DCC7D2</t>
+  </si>
+  <si>
+    <t>77AE91FCBD60CE4A1C74F96200FF1D818584813B43B0639EE6856123AB835618</t>
+  </si>
+  <si>
+    <t>9CF9F8E7EE9147429E05E9D827C4D668A40A3C9AAA441D248C335EC23DAD49BA</t>
+  </si>
+  <si>
+    <t>792C0BC171221A2F52315C70EF0527BABEBFCCAEB41C2FDD33F36649D06D51DB</t>
+  </si>
+  <si>
+    <t>1F4177FC3582CC9E113D295A9C61F04B994726C7C25CF9C6167F40D40239AE56</t>
+  </si>
+  <si>
+    <t>A5C2B0FC0E6313C12E0E997061A275C398C3C070ED93D405DAC152A0D93C03EF</t>
+  </si>
+  <si>
+    <t>953F6366BFEB5F16DE9C940126F97A80999EF4BC0E6A49E6732D6F1830273707</t>
+  </si>
+  <si>
+    <t>B93CCF70E1B04DA0920011FA61E6A82D7FD971B26A81989A25DCB8968698D5BA</t>
+  </si>
+  <si>
+    <t>EE7C24CAEC89619E5D419220CFCAC67375D9E65A266CE7683D6A8C669B5520AF</t>
+  </si>
+  <si>
+    <t>3694620746A96605B26036338539CCCED7B229B7E325F8FA8B08617BDFD4C63C</t>
+  </si>
+  <si>
+    <t>75AAF23211CA80B2E8862A4E6510ECD9A82F6F380EEE1C96F327EB8E45181C7E</t>
+  </si>
+  <si>
+    <t>DC4F8A75F99A332EBF637417042C951DCB943F31DCB70BB88240D8AB01147482</t>
+  </si>
+  <si>
+    <t>B40A331E8DE7F4AA21D284D148A794E3880C0355ED50EC25835FC34AB4C4145C</t>
+  </si>
+  <si>
+    <t>12C4AC3FA14DA50F4A4D28E6C272C43419475524EA00551DE797051ACE952712</t>
+  </si>
+  <si>
+    <t>EE43ED848FFD8B81A8D53698A2C659B887D0297EAE75E70E1D3FD8862958166E</t>
+  </si>
+  <si>
+    <t>CE8D8EA76A134E813BEE1811436A7849EF6FB0606F42CA0F8CC682EE22700B47</t>
+  </si>
+  <si>
+    <t>D5F7A5B6503D7BC195CEADBB41D709D285A30B34412D807AB4A4DC715A5B6B47</t>
+  </si>
+  <si>
+    <t>579F7076C8F992FAB326D4FE43FA54A291567CE97599DBB120EF0A05CBDED43F</t>
+  </si>
+  <si>
+    <t>023143FD46C7D3DBE3CBA9726C64EA8C0F39CAD4BB7E700764C5F793727A36DC</t>
+  </si>
+  <si>
+    <t>0603FC63B184026EA43D77DBB10DCF2A433B55B71F745E4DC3AD38A33F154CB6</t>
+  </si>
+  <si>
+    <t>5D6FE48872CCBA6B110313873049C3C9576C0222691EFF7F88A7F335A480C363</t>
+  </si>
+  <si>
+    <t>E867CA567AE6467DDC9AD3706B90115471F1578B3302DE45107DC951A8D4CC5F</t>
+  </si>
+  <si>
+    <t>8DC6A55F0C1D7694F819C216532B8585BD9D1173EACAA97A4D863DD854CE9E1C</t>
+  </si>
+  <si>
+    <t>5A8D3E2C5BEDBDC02615E4E6530DFCB5D8FBE8375F1A85AD95B90E91BFBF49D2</t>
+  </si>
+  <si>
+    <t>C3389FC8997D37D37CF69EB8F882CC341532CA0D88DE6F40046FC6813379CC5A</t>
+  </si>
+  <si>
+    <t>9FD47C321AD6FAB6B02FE584438FD4DE04A2B48265738EB473C912A94D6E0DB3</t>
+  </si>
+  <si>
+    <t>ED071A0346A021DCD08153F9F11DB212C0D478EE4ED445330AE74918AD31E668</t>
+  </si>
+  <si>
+    <t>00CFCD97F4F0DA397BC3FFEB1F0020FDCCBF01CDC1EC01C4593454E2791384D2</t>
+  </si>
+  <si>
+    <t>0531FE873F2542EDDB0F1190883DA307AF372E887F699FAC78E4863252CB28D6</t>
+  </si>
+  <si>
+    <t>2EA0F6A613C4453443DBD998507C2008A507F134DDFC9A828D11C761FC3FB5E7</t>
+  </si>
+  <si>
+    <t>4D8FB04964A676586101782C64E81648314B97C33FF5D41AFD292A8BE8765D33</t>
+  </si>
+  <si>
+    <t>AB051D6EB46D9C054777F4C616BBF773188C70F8E3D1B6EFF1E934F62CA710A4</t>
+  </si>
+  <si>
+    <t>ECA854D0C0DEFD6D067CE2440B78916AFE8EC250C36BD3805AD1CF1B4EB079CB</t>
+  </si>
+  <si>
+    <t>704EA6D988C912693B43153AB80EE515D681F6734B3F630AFC0B01606961FE72</t>
+  </si>
+  <si>
+    <t>FBF7A6435F076470080E7965B9221E90E222A7FE50BF53D98BDCAD30E6E45009</t>
+  </si>
+  <si>
+    <t>F20ABEA43F4D589044F21B41AD3360E2FDB45C72E75084671A42E0ACBD3CDA9E</t>
+  </si>
+  <si>
+    <t>B0539C86F2EBC8675BBB9F5228ADB73A547D741774F0A74C9CA4BCE93CBCA2C1</t>
+  </si>
+  <si>
+    <t>nftA1</t>
+  </si>
+  <si>
+    <t>nftA2</t>
+  </si>
+  <si>
+    <t>D97196A70B1CADF989963BAFB8ED8EC77D818773964E5C5A4631F252A70D70FA</t>
+  </si>
+  <si>
+    <t>AA3B48F2FBCEC7F74B74D79525083017595C34E86E9143D2B4F216AE22D31C54</t>
+  </si>
+  <si>
+    <t>E0F9CE5A6E0F918F323E7726ABBE73916F545B946030555E4C52262E9037352D</t>
+  </si>
+  <si>
+    <t>229D567DFAD95923378EFE3110FE0F2CD336BE1B923B54AD78F17B6D114E95D0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -322,6 +487,26 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -434,30 +619,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -469,7 +657,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -481,19 +669,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="3"/>
+    <cellStyle name="Обычный 3" xfId="4"/>
+    <cellStyle name="Обычный 4" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1652,20 +1853,20 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="4" width="33.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
+    <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1">
+      <c r="B3" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-    </row>
-    <row r="7" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+    </row>
+    <row r="7" spans="2:4" ht="17.399999999999999">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1676,14 +1877,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="15">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="15">
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
         <v>5</v>
@@ -1692,14 +1893,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" ht="15">
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="15">
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
         <v>5</v>
@@ -1708,14 +1909,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" ht="15">
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" ht="15">
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
         <v>5</v>
@@ -1724,14 +1925,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" ht="15">
       <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="15">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
         <v>5</v>
@@ -1740,340 +1941,340 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="15">
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="15">
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="15">
+      <c r="B19" s="2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="15">
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="15">
+      <c r="B21" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="15">
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="15">
       <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="15">
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="15">
       <c r="B25" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="15">
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="15">
       <c r="B27" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" ht="15">
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="15">
       <c r="B29" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="15">
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="15">
       <c r="B31" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" ht="15">
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="15">
       <c r="B33" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" ht="15">
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="15">
       <c r="B35" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" ht="15">
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="15">
       <c r="B37" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" ht="15">
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="15">
       <c r="B39" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" ht="15">
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="15">
       <c r="B41" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" ht="15">
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="15">
       <c r="B43" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" ht="15">
       <c r="B44" s="3"/>
       <c r="C44" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="15">
       <c r="B45" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" ht="15">
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="15">
       <c r="B47" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" ht="15">
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" ht="15">
       <c r="B49" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" ht="15">
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="15">
       <c r="B51" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" ht="15">
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="15">
       <c r="B53" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" ht="15">
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" ht="15">
       <c r="B55" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" ht="15">
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" ht="15">
       <c r="B57" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" ht="15">
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2115,16 +2316,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="14" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="14" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2135,67 +2338,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="46" t="s">
+        <v>71</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2215,16 +2418,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="15" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="15" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2235,67 +2440,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="46" t="s">
+        <v>72</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2315,16 +2520,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="16" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="16" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2335,67 +2542,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="46" t="s">
+        <v>73</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2415,16 +2622,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="17" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="17" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2435,67 +2644,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="46" t="s">
+        <v>74</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2515,16 +2724,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="18" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="18" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2535,67 +2746,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="46" t="s">
+        <v>75</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2615,16 +2826,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="19" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="19" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2635,71 +2848,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>76</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>59</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>77</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>60</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>78</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>61</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>60</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2719,16 +2940,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="21" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="21" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2739,71 +2962,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>80</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>59</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>81</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>61</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>82</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>62</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>61</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2823,16 +3054,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="22" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="22" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2843,71 +3076,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>84</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>59</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>85</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>63</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>86</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>61</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>63</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2927,16 +3168,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="23" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="23" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2947,71 +3190,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>88</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>59</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>89</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>63</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>90</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>60</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>63</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3031,16 +3282,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="24" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="24" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3051,71 +3304,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>92</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>59</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>60</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>94</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>63</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>60</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3136,10 +3397,10 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14.6640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" style="5" customWidth="1"/>
@@ -3152,7 +3413,7 @@
     <col min="10" max="16384" width="12.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -3178,31 +3439,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H2" s="32"/>
     </row>
-    <row r="3" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -3212,7 +3473,7 @@
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -3222,7 +3483,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -3232,7 +3493,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -3242,7 +3503,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -3252,7 +3513,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -3262,7 +3523,7 @@
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -3272,7 +3533,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3295,16 +3556,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="25" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="25" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3315,71 +3578,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>96</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>59</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>97</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>62</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>98</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>61</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>62</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3399,16 +3670,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="26" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="26" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3419,71 +3692,87 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>100</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>59</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>101</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>60</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>102</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>63</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>61</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>63</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>60</v>
+      </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3503,16 +3792,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="27" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="27" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3523,71 +3814,87 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>106</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>59</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>107</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>61</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>108</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>60</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>62</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>60</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>61</v>
+      </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3611,13 +3918,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="6" width="11.44140625" style="28" customWidth="1"/>
     <col min="7" max="16384" width="11.44140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3626,67 +3933,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16.350000000000001" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3707,17 +4014,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="6" width="11.44140625" style="29" customWidth="1"/>
     <col min="7" max="16384" width="11.44140625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3726,67 +4033,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3807,15 +4114,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="6" width="11.44140625" style="30" customWidth="1"/>
     <col min="7" max="16384" width="11.44140625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3824,67 +4133,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3905,15 +4214,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="6" width="11.44140625" style="31" customWidth="1"/>
     <col min="7" max="16384" width="11.44140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3922,67 +4233,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>116</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3999,22 +4310,117 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
+  <cols>
+    <col min="1" max="6" width="11.44140625" style="31" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
     <col min="3" max="6" width="12.6640625" style="35" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4025,60 +4431,60 @@
       <c r="D1" s="34"/>
       <c r="E1" s="34"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4102,7 +4508,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
     <col min="3" max="3" width="16" style="35" customWidth="1"/>
@@ -4110,7 +4516,7 @@
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4123,68 +4529,68 @@
       <c r="D1" s="33"/>
       <c r="E1" s="34"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>62</v>
+        <v>119</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4205,10 +4611,10 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
     <col min="3" max="3" width="16" style="35" customWidth="1"/>
@@ -4216,7 +4622,7 @@
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4231,64 +4637,64 @@
       </c>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4309,10 +4715,10 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
     <col min="3" max="3" width="16" style="35" customWidth="1"/>
@@ -4320,7 +4726,7 @@
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4335,64 +4741,64 @@
       </c>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>66</v>
+        <v>122</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4413,10 +4819,10 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
     <col min="3" max="3" width="16" style="35" customWidth="1"/>
@@ -4424,7 +4830,7 @@
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4439,64 +4845,64 @@
       </c>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>68</v>
+        <v>124</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4520,7 +4926,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="17.88671875" style="35" customWidth="1"/>
     <col min="2" max="2" width="16" style="35" customWidth="1"/>
@@ -4530,7 +4936,7 @@
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4545,64 +4951,64 @@
       </c>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4622,16 +5028,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="13" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="13" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -4642,67 +5050,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>21</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>64</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>

</xml_diff>